<commit_message>
Updated README, a few updates to sample data set
</commit_message>
<xml_diff>
--- a/test_data/sample/CATALOG_sample.xlsx
+++ b/test_data/sample/CATALOG_sample.xlsx
@@ -8,7 +8,7 @@
     <sheet name="People" sheetId="3" r:id="rId3"/>
     <sheet name="Equipment" sheetId="4" r:id="rId4"/>
     <sheet name="Places" sheetId="5" r:id="rId5"/>
-    <sheet name="Organisations" sheetId="6" r:id="rId6"/>
+    <sheet name="Organizations" sheetId="6" r:id="rId6"/>
     <sheet name="Licenses" sheetId="7" r:id="rId7"/>
     <sheet name="Publications" sheetId="8" r:id="rId8"/>
     <sheet name="Projects" sheetId="9" r:id="rId9"/>
@@ -517,7 +517,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Files"/>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -534,9 +534,6 @@
       </c>
       <c r="D1" t="str">
         <v>License</v>
-      </c>
-      <c r="E1" t="str">
-        <v>*MISSING-FILE*</v>
       </c>
     </row>
   </sheetData>
@@ -627,7 +624,7 @@
         <v>URL</v>
       </c>
       <c r="E1" t="str">
-        <v>TYPE</v>
+        <v>TYPE:</v>
       </c>
     </row>
     <row r="2">
@@ -714,7 +711,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Organisations"/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -750,10 +747,27 @@
         <v>Broadway, 2007, NSW Australia</v>
       </c>
       <c r="F2" t="str">
-        <v>Organisation</v>
+        <v>Organization</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>http://ands.org.au</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Australian National Data Service</v>
+      </c>
+      <c r="C3" t="str">
+        <v>The core purpose iof the Australian National Data Service (ANDS) is to make Australia’s research data assets more valuable for researchers, research institutions and the nation.</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Organization</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
 </worksheet>
 </file>
@@ -761,93 +775,6 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Licenses"/>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Description</v>
-      </c>
-    </row>
-    <row r="2" xml:space="preserve">
-      <c r="A2" t="str">
-        <v>https://creativecommons.org/licenses/by-nc-sa/3.0/au/</v>
-      </c>
-      <c r="B2" t="str">
-        <v>CC BY-NC-SA 3.0 AU</v>
-      </c>
-      <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Attribution-NonCommercial-ShareAlike 3.0 Australia (CC BY-NC-SA 3.0 AU)_x000d_
-_x000d_
-_x000d_
-_x000d_
-This is a human-readable summary of (and not a substitute for) the license. Disclaimer._x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-You are free to:_x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-Share — copy and redistribute the material in any medium or format_x000d_
-_x000d_
-_x000d_
-_x000d_
-Adapt — remix, transform, and build upon the material_x000d_
-_x000d_
-_x000d_
-_x000d_
-The licensor cannot revoke these freedoms as long as you follow the license terms._x000d_
-_x000d_
-_x000d_
-_x000d_
-Under the following terms:_x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-_x000d_
-Attribution — You must give appropriate credit, provide a link to the license, and indicate if changes were made. You may do so in any reasonable manner, but not in any way that suggests the licensor endorses you or your use._x000d_
-_x000d_
-_x000d_
-_x000d_
-Non-Commercial — You may not use the material for commercial purposes._x000d_
-_x000d_
-_x000d_
-_x000d_
-ShareAlike — If you remix, transform, or build upon the material, you must distribute your contributions under the same license as the original._x000d_
-_x000d_
-_x000d_
-_x000d_
-No additional restrictions — You may not apply legal terms or technological measures that legally restrict others from doing anything the license permits.</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Publications"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -858,40 +785,138 @@
         <v>ID</v>
       </c>
       <c r="B1" t="str">
-        <v>Title</v>
+        <v>Name</v>
       </c>
       <c r="C1" t="str">
-        <v>DC:CREATOR*</v>
+        <v>Description</v>
       </c>
       <c r="D1" t="str">
         <v>TYPE:</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>http://dx.doi.org/10.1000/123456</v>
+        <v>https://creativecommons.org/licenses/by-nc-sa/3.0/au/</v>
       </c>
       <c r="B2" t="str">
-        <v>This is an example publication with a dodgy DOI</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Peter Sefton</v>
-      </c>
-      <c r="D2" t="str">
-        <v>ScholarlyWork</v>
+        <v>CC BY-NC-SA 3.0 AU</v>
+      </c>
+      <c r="C2" t="str" xml:space="preserve">
+        <v xml:space="preserve">Attribution-NonCommercial-ShareAlike 3.0 Australia (CC BY-NC-SA 3.0 AU)_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+This is a human-readable summary of (and not a substitute for) the license. Disclaimer._x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+You are free to:_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+Share — copy and redistribute the material in any medium or format_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+Adapt — remix, transform, and build upon the material_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+The licensor cannot revoke these freedoms as long as you follow the license terms._x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+Under the following terms:_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+Attribution — You must give appropriate credit, provide a link to the license, and indicate if changes were made. You may do so in any reasonable manner, but not in any way that suggests the licensor endorses you or your use._x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+Non-Commercial — You may not use the material for commercial purposes._x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+ShareAlike — If you remix, transform, or build upon the material, you must distribute your contributions under the same license as the original._x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+_x000d_
+No additional restrictions — You may not apply legal terms or technological measures that legally restrict others from doing anything the license permits.</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Projects"/>
+  <sheetPr codeName="Publications"/>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -905,10 +930,60 @@
         <v>Name</v>
       </c>
       <c r="C1" t="str">
+        <v>RELATION:Creator*</v>
+      </c>
+      <c r="D1" t="str">
+        <v>TYPE:</v>
+      </c>
+      <c r="E1" t="str">
+        <v>datePublished</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>http://dx.doi.org/10.1000/123456</v>
+      </c>
+      <c r="B2" t="str">
+        <v>This is an example publication with a dodgy DOI</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Peter Sefton</v>
+      </c>
+      <c r="D2" t="str">
+        <v>ScholarlyArticle</v>
+      </c>
+      <c r="E2">
+        <v>2018</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Projects"/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="C1" t="str">
         <v>Description</v>
       </c>
       <c r="D1" t="str">
-        <v>RELATION:Funder</v>
+        <v>RELATION:Funder*</v>
       </c>
       <c r="E1" t="str">
         <v>TYPE:</v>
@@ -916,13 +991,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>https://github.com/UTS-eResearch/datacrate</v>
+        <v>https://github.com/UTS-eResearch/projects/datacrate</v>
       </c>
       <c r="B2" t="str">
-        <v>DataCrate</v>
+        <v>DataCrate Project</v>
       </c>
       <c r="C2" t="str">
-        <v>The DataCrate project is to write the spec for DataCrate, of which this is an example.</v>
+        <v>The DataCrate project is to write the spec for DataCrate, of which this is an example. The DataCrate project is part of the University of Technology Sydney's Provisioner project.</v>
       </c>
       <c r="D2" t="str">
         <v>University of Technology Sydney</v>
@@ -931,7 +1006,28 @@
         <v>Project</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>http://eresearch.uts.edu.au/projects/provisioner</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Provisioner</v>
+      </c>
+      <c r="C3" t="str">
+        <v xml:space="preserve">The University of Technology Sydney Provisioner project is </v>
+      </c>
+      <c r="D3" t="str">
+        <v>University of Technology Sydney, Australian National Data Service</v>
+      </c>
+      <c r="E3" t="str">
+        <v xml:space="preserve">Project </v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
 </worksheet>
 </file>
</xml_diff>